<commit_message>
new database in schedule
</commit_message>
<xml_diff>
--- a/res/bd/schedule/database.xlsx
+++ b/res/bd/schedule/database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t xml:space="preserve">day</t>
   </si>
@@ -49,13 +49,13 @@
     <t xml:space="preserve">кінець</t>
   </si>
   <si>
-    <t xml:space="preserve">first couple</t>
+    <t xml:space="preserve">240р, Фізика, лекція, доцент Олійник Сергій Володимирович</t>
   </si>
   <si>
     <t xml:space="preserve">https://</t>
   </si>
   <si>
-    <t xml:space="preserve">мастер к</t>
+    <t xml:space="preserve">доцент Олійник Сергій Володимирович</t>
   </si>
   <si>
     <t xml:space="preserve">maincraft</t>
@@ -64,7 +64,85 @@
     <t xml:space="preserve">ч</t>
   </si>
   <si>
+    <t xml:space="preserve">343г, Мовні компетентності, практика,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> асистент Федотова Олена Михайлівна</t>
+  </si>
+  <si>
     <t xml:space="preserve">з</t>
+  </si>
+  <si>
+    <t xml:space="preserve">416р, Фізика, практика, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фізичне виховання, практика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240р, Фізика, лекція,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> доцент Олійник Сергій Володимирович</t>
+  </si>
+  <si>
+    <t xml:space="preserve">102р, Алгоритми і структури даних, лекція, доцент Єремеєв Олег Ігорович</t>
+  </si>
+  <si>
+    <t xml:space="preserve">доцент Єремеєв Олег Ігорович</t>
+  </si>
+  <si>
+    <t xml:space="preserve">207лк, Вища математика, лекція, професор Курєннов Сергій Сергійович</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> професор Курєннов Сергій Сергійович</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101р, UNIX-подібні операційні системи (Адмін. інфоком. систем, Операц. с-ми мед. прогр. компл.), лекція, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">доцент Зряхов Михайло Сергійович</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311р, UNIX-подібні ОС; Адмін. інф. сист., практика, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">409лк, Вища математика, практика, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">старший викладач Томілова Євгенія Павлівна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">410г, Правова компетентність, лекція, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">доцент Голубов Артем Євгенович</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101р, Основи програмування, лекція, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">доцент Рубель Олексій Сергійович</t>
+  </si>
+  <si>
+    <t xml:space="preserve">315р, Алгоритми і структури даних, практика, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">205лк, Вища математика, лекція,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">427г, Правова компетентність, лекція, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">315р, Основи програмування, практика,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> старший викладач Рубель Андрій Сергійович</t>
+  </si>
+  <si>
+    <t xml:space="preserve">348г, Мовні компетентності, практика, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">асистент Федотова Олена Михайлівна</t>
   </si>
 </sst>
 </file>
@@ -75,7 +153,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -111,6 +189,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="5">
@@ -173,7 +257,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -194,6 +278,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -203,6 +291,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -283,21 +375,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10:L10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="78.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="3.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="8.67"/>
   </cols>
@@ -344,7 +436,7 @@
       <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -356,10 +448,10 @@
       <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="5" t="n">
+      <c r="K2" s="6" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="L2" s="5" t="n">
+      <c r="L2" s="6" t="n">
         <v>0.399305555555556</v>
       </c>
     </row>
@@ -370,35 +462,46 @@
       <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D3" s="4"/>
+      <c r="E3" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="G3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="K3" s="6" t="n">
         <v>0.409722222222222</v>
       </c>
-      <c r="L3" s="5" t="n">
+      <c r="L3" s="6" t="n">
         <v>0.475694444444444</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="G4" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="5" t="n">
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="6" t="n">
         <v>0.496527777777778</v>
       </c>
-      <c r="L4" s="5" t="n">
+      <c r="L4" s="6" t="n">
         <v>0.5625</v>
       </c>
     </row>
@@ -409,14 +512,16 @@
       <c r="B5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="G5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="6" t="n">
         <v>0.65</v>
       </c>
-      <c r="L5" s="5" t="n">
+      <c r="L5" s="6" t="n">
         <v>0.638888888888889</v>
       </c>
     </row>
@@ -428,7 +533,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K6" s="3" t="n">
@@ -438,39 +543,54 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="G7" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>1</v>
@@ -481,103 +601,143 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B12" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="G14" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B16" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B15" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="G17" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="G18" s="1" t="n">
         <v>1</v>
@@ -590,55 +750,81 @@
       <c r="B19" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="G19" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="n">
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="B20" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7" t="n">
+      <c r="B20" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="B21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="G22" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="G23" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>